<commit_message>
Se añadio ubicacion y atrivutos a usuarios
</commit_message>
<xml_diff>
--- a/ExtraClase/Modelado de Dominio/Modelo enriquesido/Proyecto extraclase.xlsx
+++ b/ExtraClase/Modelado de Dominio/Modelo enriquesido/Proyecto extraclase.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Federico\U\Doo\RepositorioDOO\ExtraClase\Modelado de Dominio\Modelo enriquesido\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC93AACC-E5AA-40A4-BEDE-FDB7048D3C87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{457D3C3A-D51A-4637-8912-B1A53C810727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="2" xr2:uid="{91EDD603-1B87-409C-9594-5C05F8123E08}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="4" activeTab="9" xr2:uid="{91EDD603-1B87-409C-9594-5C05F8123E08}"/>
   </bookViews>
   <sheets>
-    <sheet name="Valores" sheetId="1" r:id="rId1"/>
+    <sheet name="Valores" sheetId="1" state="hidden" r:id="rId1"/>
     <sheet name="Modelo de dominio" sheetId="2" state="hidden" r:id="rId2"/>
     <sheet name="Objeto de dominio" sheetId="3" r:id="rId3"/>
     <sheet name="Calificación" sheetId="9" r:id="rId4"/>
@@ -22,8 +22,12 @@
     <sheet name="Historia vehiculo" sheetId="11" r:id="rId7"/>
     <sheet name="Ruta" sheetId="8" r:id="rId8"/>
     <sheet name="Conductor" sheetId="6" r:id="rId9"/>
-    <sheet name="Datos simulados " sheetId="5" r:id="rId10"/>
+    <sheet name="Ubicacion" sheetId="12" r:id="rId10"/>
+    <sheet name="Datos simulados " sheetId="5" r:id="rId11"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId12"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -44,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="136">
   <si>
     <t>Tipo de dato</t>
   </si>
@@ -193,15 +197,9 @@
     <t>Federico Zapata</t>
   </si>
   <si>
-    <t>rionegroñ*</t>
-  </si>
-  <si>
     <t>Rionegro</t>
   </si>
   <si>
-    <t>federico.zapata4970@uco.net.co</t>
-  </si>
-  <si>
     <t>Datos simulados</t>
   </si>
   <si>
@@ -377,6 +375,87 @@
   </si>
   <si>
     <t>Da una guia de cuales han sido los precios para destinos similares, con la idea de poder generar un precio medio o un estimado de lo que se pueda pagar por una ruta con origen y destino igual.</t>
+  </si>
+  <si>
+    <t>Entidad que representa cual será el lugar geografico de un cliente o un conductor al momento de registrar un servicio, como lo puede ser una ciudad, barrio o sesctor. Por ejemplo un cliente puede estar en la ciudad rionegro en el barrio villa Manuela.</t>
+  </si>
+  <si>
+    <t>Con este atributo se conocera como se llama la persona que se va recoger o el conductor que hara la ruta.</t>
+  </si>
+  <si>
+    <t>Ciudad</t>
+  </si>
+  <si>
+    <t>-Quitar espacios en blanco al inicio y al final</t>
+  </si>
+  <si>
+    <t>Se sabra en cual de las ciudades es que en la vive la persona que se va recoger o cual será el origen de la ruta</t>
+  </si>
+  <si>
+    <t>Barrio o sector</t>
+  </si>
+  <si>
+    <t>Con este atributo se podra saber de una manera más exacta donde se encutra el conductor o el cliente.</t>
+  </si>
+  <si>
+    <t>Hora</t>
+  </si>
+  <si>
+    <t>Hora-Día-Mes</t>
+  </si>
+  <si>
+    <t>En caso de no poner una hora se pondra la hora actual de la zona</t>
+  </si>
+  <si>
+    <t>Atributo para saber el momento exacto en el cual se se encuentra un cliente o conductor</t>
+  </si>
+  <si>
+    <t>En caso de no poner una descripción se pondra el atributo &lt;Barrio&gt;</t>
+  </si>
+  <si>
+    <t>Atributo que indica con más exactitud en que lugar se encuentra un conductor o cliente, como lo puede ser la direccion en calles y carreras</t>
+  </si>
+  <si>
+    <t>Comentario</t>
+  </si>
+  <si>
+    <t>Longitud</t>
+  </si>
+  <si>
+    <t>Latitud</t>
+  </si>
+  <si>
+    <t>Valor actual de posición geografico</t>
+  </si>
+  <si>
+    <t>Se puede usar grados, minutos y segundos</t>
+  </si>
+  <si>
+    <t>Con este atributo representa de manera unica una ubicación de un usuario.</t>
+  </si>
+  <si>
+    <t>Ruta solicitada</t>
+  </si>
+  <si>
+    <t>Atributo que representa cuando un cliente pide una ruta, con el fin de que un conductor pueda saber que un cliente solicito la ruta creada.</t>
+  </si>
+  <si>
+    <t>Ruta realizar</t>
+  </si>
+  <si>
+    <t>Atributo que representa cuando un conductor genera una ruta, con el fin de que un cliente pueda saber que si un conductor creo una ruta.</t>
+  </si>
+  <si>
+    <t>Villa Manuela</t>
+  </si>
+  <si>
+    <t>Es la carrera DD # 40 a</t>
+  </si>
+  <si>
+    <t>Atributo que representa las coordenadas greograficas de logitud en tiempo real, estas se adquiren gracias al gps de los usuarios</t>
+  </si>
+  <si>
+    <t>Atributo que representa las coordenadas greograficas de latitud en tiempo real, estas se adquiren gracias al gps de los usuarios</t>
   </si>
 </sst>
 </file>
@@ -386,7 +465,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -431,8 +510,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -487,8 +579,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -603,13 +707,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -655,12 +783,8 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -671,12 +795,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -712,6 +830,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="44" fontId="0" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -776,6 +897,52 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="6" fillId="8" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -842,6 +1009,44 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Valores"/>
+      <sheetName val="Modelo de dominio"/>
+      <sheetName val="Objeto de domionio"/>
+      <sheetName val="Posicion"/>
+      <sheetName val="Posicion-Datos simulados"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>Objeto de dominio</v>
+          </cell>
+          <cell r="B1" t="str">
+            <v>Descripcion</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>Posición</v>
+          </cell>
+          <cell r="B2" t="str">
+            <v>Entidad que representa cual será el lugar geografico de un cliente o un conductor al momento de registrar un servicio, como lo puede ser una ciudad, barrio o sesctor. Por ejemplo un cliente puede estar en la ciudad rionegro en el barrio villa Manuela.</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1209,7 +1414,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1218,12 +1423,537 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C90D05C5-BA3B-422D-836B-B3214C52165B}">
+  <dimension ref="A1:P13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P14" sqref="P13:P14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="56.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="60.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="54.7109375" style="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="61" t="str">
+        <f>'[1]Objeto de domionio'!A1&amp;":"</f>
+        <v>Objeto de dominio:</v>
+      </c>
+      <c r="B2" s="42" t="str">
+        <f>'[1]Objeto de domionio'!A2&amp;":"</f>
+        <v>Posición:</v>
+      </c>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="44"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="61" t="str">
+        <f>'[1]Objeto de domionio'!B1&amp;":"</f>
+        <v>Descripcion:</v>
+      </c>
+      <c r="B3" s="62" t="str">
+        <f>'[1]Objeto de domionio'!B2</f>
+        <v>Entidad que representa cual será el lugar geografico de un cliente o un conductor al momento de registrar un servicio, como lo puede ser una ciudad, barrio o sesctor. Por ejemplo un cliente puede estar en la ciudad rionegro en el barrio villa Manuela.</v>
+      </c>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="62"/>
+      <c r="K3" s="62"/>
+      <c r="L3" s="62"/>
+      <c r="M3" s="62"/>
+      <c r="N3" s="62"/>
+      <c r="O3" s="62"/>
+      <c r="P3" s="62"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="63"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="63"/>
+      <c r="K4" s="63"/>
+      <c r="L4" s="63"/>
+      <c r="M4" s="63"/>
+      <c r="N4" s="63"/>
+      <c r="O4" s="63"/>
+      <c r="P4" s="64"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="70" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="66" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="69"/>
+      <c r="D6" s="69"/>
+      <c r="E6" s="69"/>
+      <c r="F6" s="69"/>
+      <c r="G6" s="69"/>
+      <c r="H6" s="69"/>
+      <c r="I6" s="69"/>
+      <c r="J6" s="69"/>
+      <c r="K6" s="65" t="s">
+        <v>4</v>
+      </c>
+      <c r="L6" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="M6" s="65" t="s">
+        <v>4</v>
+      </c>
+      <c r="N6" s="65" t="s">
+        <v>4</v>
+      </c>
+      <c r="O6" s="65" t="s">
+        <v>4</v>
+      </c>
+      <c r="P6" s="71" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="65" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="66" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="65">
+        <v>1</v>
+      </c>
+      <c r="D7" s="65">
+        <v>50</v>
+      </c>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="65" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" s="65"/>
+      <c r="J7" s="65"/>
+      <c r="K7" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="L7" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="M7" s="65" t="s">
+        <v>4</v>
+      </c>
+      <c r="N7" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="O7" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="P7" s="67" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="65" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8" s="66" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="65">
+        <v>4</v>
+      </c>
+      <c r="D8" s="65">
+        <v>20</v>
+      </c>
+      <c r="E8" s="65"/>
+      <c r="F8" s="65"/>
+      <c r="G8" s="65"/>
+      <c r="H8" s="65" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8" s="65"/>
+      <c r="J8" s="68" t="s">
+        <v>112</v>
+      </c>
+      <c r="K8" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="L8" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="M8" s="65" t="s">
+        <v>4</v>
+      </c>
+      <c r="N8" s="65" t="s">
+        <v>4</v>
+      </c>
+      <c r="O8" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="P8" s="67" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="65" t="s">
+        <v>114</v>
+      </c>
+      <c r="B9" s="66" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="65">
+        <v>2</v>
+      </c>
+      <c r="D9" s="65">
+        <v>40</v>
+      </c>
+      <c r="E9" s="65"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="65"/>
+      <c r="H9" s="65" t="s">
+        <v>38</v>
+      </c>
+      <c r="I9" s="65"/>
+      <c r="J9" s="68" t="s">
+        <v>112</v>
+      </c>
+      <c r="K9" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="L9" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="M9" s="65" t="s">
+        <v>4</v>
+      </c>
+      <c r="N9" s="65" t="s">
+        <v>4</v>
+      </c>
+      <c r="O9" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="P9" s="67" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="65" t="s">
+        <v>116</v>
+      </c>
+      <c r="B10" s="66" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="65"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="65"/>
+      <c r="H10" s="65" t="s">
+        <v>117</v>
+      </c>
+      <c r="I10" s="65" t="s">
+        <v>118</v>
+      </c>
+      <c r="J10" s="65"/>
+      <c r="K10" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="L10" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="M10" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="N10" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="O10" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="P10" s="67" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="65" t="s">
+        <v>123</v>
+      </c>
+      <c r="B11" s="66" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="28">
+        <v>10</v>
+      </c>
+      <c r="D11" s="28">
+        <v>200</v>
+      </c>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="J11" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="K11" s="65" t="s">
+        <v>4</v>
+      </c>
+      <c r="L11" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="M11" s="65" t="s">
+        <v>4</v>
+      </c>
+      <c r="N11" s="65" t="s">
+        <v>4</v>
+      </c>
+      <c r="O11" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="P11" s="29" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="65" t="s">
+        <v>124</v>
+      </c>
+      <c r="B12" s="66" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="28">
+        <v>10</v>
+      </c>
+      <c r="D12" s="28">
+        <v>200</v>
+      </c>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="I12" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="J12" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="K12" s="65" t="s">
+        <v>4</v>
+      </c>
+      <c r="L12" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="M12" s="65" t="s">
+        <v>4</v>
+      </c>
+      <c r="N12" s="65" t="s">
+        <v>4</v>
+      </c>
+      <c r="O12" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="P12" s="29" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="65" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="66" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="65">
+        <v>0</v>
+      </c>
+      <c r="D13" s="65">
+        <v>100</v>
+      </c>
+      <c r="E13" s="65"/>
+      <c r="F13" s="65"/>
+      <c r="G13" s="65"/>
+      <c r="H13" s="65" t="s">
+        <v>39</v>
+      </c>
+      <c r="I13" s="65" t="s">
+        <v>120</v>
+      </c>
+      <c r="J13" s="65"/>
+      <c r="K13" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="L13" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="M13" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="N13" s="65" t="s">
+        <v>4</v>
+      </c>
+      <c r="O13" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="P13" s="67" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B2:P2"/>
+    <mergeCell ref="B3:P3"/>
+    <mergeCell ref="A1:P1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A4" location="'Datos simulados '!A1" display="Datos simulados" xr:uid="{B4BAE432-FE88-43E7-BFE7-04FC3AC6E54F}"/>
+    <hyperlink ref="A1:P1" location="'Objeto de dominio'!A1" display="Volver al inicio!A1" xr:uid="{4E61C635-B515-4932-98E0-92B5B3D6D8A2}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{38FDE4E7-21CD-4B2A-956A-A00A54B75CC8}">
+          <x14:formula1>
+            <xm:f>Valores!$A$2:$A$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>B6:B10 B11:B13</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C148781E-ED72-408F-A6E0-4F0BFB0D4D3F}">
+          <x14:formula1>
+            <xm:f>Valores!$B$2:$B$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>K6:O10 K11:O13</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47EE630E-1BB6-4D1A-9784-D8629178E0AB}">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1231,78 +1961,121 @@
     <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29"/>
+      <c r="A1" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="str">
+      <c r="A2" s="72" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="72"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="str">
         <f>Cliente!A6</f>
         <v>Codigo</v>
       </c>
-      <c r="B2" s="18" t="str">
+      <c r="B3" s="17" t="str">
         <f>Cliente!A7</f>
         <v>Nombre</v>
       </c>
-      <c r="C2" s="18" t="str">
-        <f>Cliente!A8</f>
-        <v>Contraseña</v>
-      </c>
-      <c r="D2" s="18" t="str">
-        <f>Cliente!A9</f>
-        <v>Posicion</v>
-      </c>
-      <c r="E2" s="18" t="str">
-        <f>Cliente!A10</f>
-        <v>Correo Entidad</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="19">
+      <c r="C3" s="17" t="str">
+        <f>Ubicacion!A8</f>
+        <v>Ciudad</v>
+      </c>
+      <c r="D3" s="17" t="str">
+        <f>Ubicacion!A9</f>
+        <v>Barrio o sector</v>
+      </c>
+      <c r="E3" s="73" t="str">
+        <f>Ubicacion!A10</f>
+        <v>Hora</v>
+      </c>
+      <c r="F3" s="75" t="str">
+        <f>Ubicacion!A11</f>
+        <v>Longitud</v>
+      </c>
+      <c r="G3" s="75" t="str">
+        <f>Ubicacion!A12</f>
+        <v>Latitud</v>
+      </c>
+      <c r="H3" s="75" t="str">
+        <f>Ubicacion!A13</f>
+        <v>Descripcion</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="18">
         <v>1</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B4" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C4" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>51</v>
+      <c r="D4" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="E4" s="74">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="76" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:E2"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A2" location="Cliente!A6" display="Cliente!A6" xr:uid="{81DC788B-B7FC-4ABD-B06A-1F7891900FB6}"/>
-    <hyperlink ref="B2" location="Cliente!A7" display="Cliente!A7" xr:uid="{BE64C897-DB76-43C5-B2FE-A0526CD92F64}"/>
-    <hyperlink ref="C2" location="'Cliente-Datos simulados '!A8" display="'Cliente-Datos simulados '!A8" xr:uid="{63494C14-9708-4AAE-908F-315C67C0B3FA}"/>
-    <hyperlink ref="D2" location="Cliente!A9" display="Cliente!A9" xr:uid="{5E004E1B-C44F-43C6-A04E-341B83594D25}"/>
-    <hyperlink ref="E2" location="Cliente!A10" display="Cliente!A10" xr:uid="{9926B372-A42D-4B36-8FD3-1BB57937B25A}"/>
-    <hyperlink ref="E3" r:id="rId1" xr:uid="{E06FAA49-298A-4BC3-8B04-A91633353EDA}"/>
+    <hyperlink ref="A3" location="Ubicacion!A6" display="Ubicacion!A6" xr:uid="{81DC788B-B7FC-4ABD-B06A-1F7891900FB6}"/>
+    <hyperlink ref="B3" location="Ubicacion!A7" display="Ubicacion!A7" xr:uid="{BE64C897-DB76-43C5-B2FE-A0526CD92F64}"/>
     <hyperlink ref="A1" location="'Objeto de dominio'!A1" display="Volver a inicio" xr:uid="{EE7ACA56-775A-4B47-9625-A8FE675C781B}"/>
+    <hyperlink ref="C3" location="Ubicacion!A8" display="Ubicacion!A8" xr:uid="{933C1983-4F97-4A3E-820D-F87A27679ECD}"/>
+    <hyperlink ref="D3" location="Ubicacion!A9" display="Ubicacion!A9" xr:uid="{3C067DB5-922C-417A-A2F2-212AF9BA81C7}"/>
+    <hyperlink ref="E3" location="Ubicacion!A10" display="Ubicacion!A10" xr:uid="{E7C0D031-DE0F-48E9-90FC-5406530517FF}"/>
+    <hyperlink ref="F3" location="Ubicacion!A11" display="Ubicacion!A11" xr:uid="{900DD669-75C5-49DF-864B-3CA3EC68B41C}"/>
+    <hyperlink ref="G3" location="Ubicacion!A12" display="Ubicacion!A12" xr:uid="{5798DF0F-FB39-4258-AB8E-D2A7EE05A8C2}"/>
+    <hyperlink ref="H3" location="Ubicacion!A13" display="Ubicacion!A13" xr:uid="{C6189213-CAA3-4B56-A8BC-CD07A884EE9A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1328,11 +2101,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA3A2587-FA68-46BD-83B7-0F0FB56FF0F2}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
+    <sheetView topLeftCell="A4" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1349,51 +2120,59 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>60</v>
+      <c r="A3" s="60" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="23" t="s">
+    </row>
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="24" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="B5" s="24" t="s">
+      <c r="B6" s="22" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
-        <v>78</v>
-      </c>
-      <c r="B6" s="24" t="s">
-        <v>79</v>
-      </c>
-    </row>
     <row r="7" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>104</v>
+      <c r="A7" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1404,6 +2183,7 @@
     <hyperlink ref="A2" location="Cliente!A2" display="Clientes" xr:uid="{B6916CA9-20CB-42CE-8010-FA8E90708088}"/>
     <hyperlink ref="A3" location="Conductor!A2" display="Conductor" xr:uid="{4F62340F-4713-464D-82E1-732835F3A9BB}"/>
     <hyperlink ref="A7" location="Ruta!A1" display="Ruta" xr:uid="{47168308-469A-4172-8A3C-E0B1CB53172C}"/>
+    <hyperlink ref="A8" location="Ubicacion!A1" display="Ubicación" xr:uid="{6B2D2F9A-3124-470D-B653-69FCCCBA7817}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1411,10 +2191,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FECAE0DE-2747-4E64-8328-AC22EB569096}">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:P4"/>
+      <selection sqref="A1:P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1439,92 +2219,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
-      <c r="O1" s="42"/>
-      <c r="P1" s="42"/>
+      <c r="A1" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="str">
         <f>'Objeto de dominio'!A1&amp;":"</f>
         <v>Objeto de dominio:</v>
       </c>
-      <c r="B2" s="40" t="str">
+      <c r="B2" s="37" t="str">
         <f>'Objeto de dominio'!A4</f>
         <v>Calificación</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="str">
         <f>'Objeto de dominio'!B1&amp;":"</f>
         <v>Descripcion:</v>
       </c>
-      <c r="B3" s="41" t="str">
+      <c r="B3" s="38" t="str">
         <f>'Objeto de dominio'!B4</f>
         <v>Entidad que representa cual es la calificacion conforme al servicio que recibio por parte del conductor, esta calificacion es general, toma en cuenta la actitud del conductor principalmente.</v>
       </c>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="41"/>
-      <c r="M3" s="41"/>
-      <c r="N3" s="41"/>
-      <c r="O3" s="41"/>
-      <c r="P3" s="41"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38"/>
+      <c r="O3" s="38"/>
+      <c r="P3" s="38"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="43"/>
-      <c r="L4" s="43"/>
-      <c r="M4" s="43"/>
-      <c r="N4" s="43"/>
-      <c r="O4" s="43"/>
-      <c r="P4" s="43"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="40"/>
+      <c r="P4" s="40"/>
     </row>
     <row r="5" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -1578,7 +2358,7 @@
     </row>
     <row r="6" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>3</v>
@@ -1593,34 +2373,34 @@
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
       <c r="H6" s="10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I6" s="10"/>
       <c r="J6" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="L6" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="M6" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="O6" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="P6" s="22" t="s">
         <v>82</v>
-      </c>
-      <c r="K6" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="L6" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="M6" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="N6" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="O6" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="P6" s="24" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>6</v>
@@ -1635,7 +2415,7 @@
         <v>5</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
@@ -1654,15 +2434,15 @@
       <c r="O7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="P7" s="24" t="s">
-        <v>87</v>
+      <c r="P7" s="22" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" s="21" t="str">
+        <v>57</v>
+      </c>
+      <c r="B8" s="19" t="str">
         <f>'Objeto de dominio'!$A$3</f>
         <v>Conductor</v>
       </c>
@@ -1672,7 +2452,7 @@
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
       <c r="H8" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
@@ -1691,15 +2471,15 @@
       <c r="O8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="P8" s="24" t="s">
-        <v>89</v>
+      <c r="P8" s="22" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="B9" s="21" t="str">
+        <v>88</v>
+      </c>
+      <c r="B9" s="19" t="str">
         <f>'Objeto de dominio'!$A$2</f>
         <v>Clientes</v>
       </c>
@@ -1709,7 +2489,7 @@
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
       <c r="H9" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
@@ -1728,8 +2508,48 @@
       <c r="O9" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="P9" s="24" t="s">
-        <v>92</v>
+      <c r="P9" s="22" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="10">
+        <v>0</v>
+      </c>
+      <c r="D10" s="10">
+        <v>100</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="L10" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="M10" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="N10" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="O10" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="P10" s="22" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1755,7 +2575,7 @@
           <x14:formula1>
             <xm:f>Valores!$A$2:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>B6:B7</xm:sqref>
+          <xm:sqref>B6:B7 B10</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1765,11 +2585,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8098E073-6F5C-467A-BA9E-712D8A189F43}">
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O10" sqref="O10"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1794,92 +2614,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
-      <c r="O1" s="42"/>
-      <c r="P1" s="42"/>
+      <c r="A1" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="str">
         <f>'Objeto de dominio'!A1&amp;":"</f>
         <v>Objeto de dominio:</v>
       </c>
-      <c r="B2" s="45" t="str">
+      <c r="B2" s="42" t="str">
         <f>'Objeto de dominio'!A2&amp;":"</f>
         <v>Clientes:</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="47"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="44"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="str">
         <f>'Objeto de dominio'!B1&amp;":"</f>
         <v>Descripcion:</v>
       </c>
-      <c r="B3" s="44" t="str">
+      <c r="B3" s="41" t="str">
         <f>'Objeto de dominio'!B2</f>
         <v>Entidad que representa a un tipo de usuario, el cual es quien solicita el servicio de carro compartido. Por ejmeplo es quien contacta con un conductor para llegar a un destino en común.</v>
       </c>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
-      <c r="N3" s="44"/>
-      <c r="O3" s="44"/>
-      <c r="P3" s="44"/>
-    </row>
-    <row r="4" spans="1:16" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="48" t="s">
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
+      <c r="N3" s="41"/>
+      <c r="O3" s="41"/>
+      <c r="P3" s="41"/>
+    </row>
+    <row r="4" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="49"/>
-      <c r="L4" s="49"/>
-      <c r="M4" s="49"/>
-      <c r="N4" s="49"/>
-      <c r="O4" s="49"/>
-      <c r="P4" s="49"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
+      <c r="M4" s="46"/>
+      <c r="N4" s="46"/>
+      <c r="O4" s="46"/>
+      <c r="P4" s="46"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -2129,6 +2949,44 @@
       </c>
       <c r="P10" s="7" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="P11" s="7" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2150,13 +3008,13 @@
           <x14:formula1>
             <xm:f>Valores!$A$2:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>B6:B10</xm:sqref>
+          <xm:sqref>B6:B11</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FD3A2786-2296-4CB8-A941-3D7305A18AEA}">
           <x14:formula1>
             <xm:f>Valores!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>K6:O10</xm:sqref>
+          <xm:sqref>K6:O11</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2193,92 +3051,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51"/>
-      <c r="P1" s="51"/>
+      <c r="A1" s="48" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+      <c r="P1" s="48"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="str">
         <f>'Objeto de dominio'!A1&amp;":"</f>
         <v>Objeto de dominio:</v>
       </c>
-      <c r="B2" s="52" t="str">
+      <c r="B2" s="49" t="str">
         <f>'Objeto de dominio'!A5</f>
         <v>Vehiculo</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="52"/>
-      <c r="P2" s="52"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="str">
         <f>'Objeto de dominio'!B1&amp;":"</f>
         <v>Descripcion:</v>
       </c>
-      <c r="B3" s="52" t="str">
+      <c r="B3" s="49" t="str">
         <f>'Objeto de dominio'!B5</f>
         <v>Entidad que se encarga de identificar al vehiculo del conductor y a su vez el dueño</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="52"/>
-      <c r="M3" s="52"/>
-      <c r="N3" s="52"/>
-      <c r="O3" s="52"/>
-      <c r="P3" s="52"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="49"/>
     </row>
     <row r="4" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="43"/>
-      <c r="L4" s="43"/>
-      <c r="M4" s="43"/>
-      <c r="N4" s="43"/>
-      <c r="O4" s="43"/>
-      <c r="P4" s="43"/>
+      <c r="A4" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="40"/>
+      <c r="P4" s="40"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -2332,7 +3190,7 @@
     </row>
     <row r="6" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>3</v>
@@ -2347,53 +3205,53 @@
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
       <c r="H6" s="10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I6" s="10"/>
       <c r="J6" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="L6" s="10" t="s">
         <v>7</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="N6" s="10" t="s">
         <v>7</v>
       </c>
       <c r="O6" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="P6" s="24" t="s">
-        <v>94</v>
+        <v>81</v>
+      </c>
+      <c r="P6" s="22" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="32">
-        <v>7</v>
-      </c>
-      <c r="D7" s="32">
-        <v>7</v>
-      </c>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32" t="s">
-        <v>96</v>
-      </c>
-      <c r="I7" s="32"/>
+      <c r="C7" s="28">
+        <v>7</v>
+      </c>
+      <c r="D7" s="28">
+        <v>7</v>
+      </c>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="I7" s="28"/>
       <c r="J7" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="K7" s="10" t="s">
         <v>7</v>
@@ -2402,7 +3260,7 @@
         <v>7</v>
       </c>
       <c r="M7" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="N7" s="10" t="s">
         <v>7</v>
@@ -2410,15 +3268,15 @@
       <c r="O7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="P7" s="33" t="s">
-        <v>97</v>
+      <c r="P7" s="29" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" s="21" t="str">
+        <v>57</v>
+      </c>
+      <c r="B8" s="19" t="str">
         <f>'Objeto de dominio'!$A$3</f>
         <v>Conductor</v>
       </c>
@@ -2428,7 +3286,7 @@
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
       <c r="H8" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
@@ -2447,29 +3305,29 @@
       <c r="O8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="P8" s="24" t="s">
+      <c r="P8" s="22" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="30" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="34" t="s">
+    <row r="11" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="B10" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="34" t="s">
+      <c r="B11" s="32" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="35" t="s">
-        <v>101</v>
-      </c>
-      <c r="B11" s="36" t="s">
-        <v>102</v>
-      </c>
-      <c r="C11" s="37" t="str">
+      <c r="C11" s="33" t="str">
         <f>A7</f>
         <v>Matricula</v>
       </c>
@@ -2496,7 +3354,7 @@
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection sqref="A1:P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2520,75 +3378,75 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51"/>
-      <c r="P1" s="51"/>
+      <c r="A1" s="48" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+      <c r="P1" s="48"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="str">
         <f>'Objeto de dominio'!A1&amp;":"</f>
         <v>Objeto de dominio:</v>
       </c>
-      <c r="B2" s="52" t="str">
+      <c r="B2" s="49" t="str">
         <f>'Objeto de dominio'!A6</f>
         <v>Historico Ruta</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="52"/>
-      <c r="P2" s="52"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="str">
         <f>'Objeto de dominio'!B1&amp;":"</f>
         <v>Descripcion:</v>
       </c>
-      <c r="B3" s="52" t="str">
+      <c r="B3" s="49" t="str">
         <f>'Objeto de dominio'!B6</f>
         <v>Entidad que se encarga de guardar todo el recorrido de la ruta que hace el conductor en su vehiculo</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="52"/>
-      <c r="M3" s="52"/>
-      <c r="N3" s="52"/>
-      <c r="O3" s="52"/>
-      <c r="P3" s="52"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="49"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="34" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2644,7 +3502,7 @@
     </row>
     <row r="6" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>3</v>
@@ -2659,29 +3517,29 @@
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
       <c r="H6" s="10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I6" s="10"/>
       <c r="J6" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="L6" s="10" t="s">
         <v>7</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="N6" s="10" t="s">
         <v>7</v>
       </c>
       <c r="O6" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="P6" s="24" t="s">
-        <v>94</v>
+        <v>81</v>
+      </c>
+      <c r="P6" s="22" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -2702,8 +3560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{481DBA3A-D410-434D-9698-683C168FAD5F}">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2728,92 +3586,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
-      <c r="O1" s="42"/>
-      <c r="P1" s="42"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="str">
         <f>'Objeto de dominio'!A1&amp;":"</f>
         <v>Objeto de dominio:</v>
       </c>
-      <c r="B2" s="53" t="str">
+      <c r="B2" s="50" t="str">
         <f>'Objeto de dominio'!A2&amp;":"</f>
         <v>Clientes:</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="55"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="51"/>
+      <c r="P2" s="52"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="str">
         <f>'Objeto de dominio'!B1&amp;":"</f>
         <v>Descripcion:</v>
       </c>
-      <c r="B3" s="56" t="str">
+      <c r="B3" s="53" t="str">
         <f>'Objeto de dominio'!B7</f>
         <v>Entidad que nos representa cuales son las rutas que se da en un viaje, como lo puede ser, por donde pasa, quienes estuvieron en el viaje y hasta donde llegaron, se busca es guardar daros por seguridad de los usuarios.</v>
       </c>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="57"/>
-      <c r="N3" s="57"/>
-      <c r="O3" s="57"/>
-      <c r="P3" s="58"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="54"/>
+      <c r="P3" s="55"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="59" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60"/>
-      <c r="M4" s="60"/>
-      <c r="N4" s="60"/>
-      <c r="O4" s="60"/>
-      <c r="P4" s="61"/>
+      <c r="A4" s="56" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="57"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="57"/>
+      <c r="F4" s="57"/>
+      <c r="G4" s="57"/>
+      <c r="H4" s="57"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="57"/>
+      <c r="K4" s="57"/>
+      <c r="L4" s="57"/>
+      <c r="M4" s="57"/>
+      <c r="N4" s="57"/>
+      <c r="O4" s="57"/>
+      <c r="P4" s="58"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -2881,7 +3739,7 @@
         <v>37</v>
       </c>
       <c r="I6" s="10"/>
-      <c r="J6" s="24"/>
+      <c r="J6" s="22"/>
       <c r="K6" s="10" t="s">
         <v>7</v>
       </c>
@@ -2898,15 +3756,15 @@
         <v>4</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>59</v>
+        <v>57</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>57</v>
       </c>
       <c r="C7" s="10">
         <v>1</v>
@@ -2921,8 +3779,8 @@
         <v>38</v>
       </c>
       <c r="I7" s="10"/>
-      <c r="J7" s="24" t="s">
-        <v>53</v>
+      <c r="J7" s="22" t="s">
+        <v>51</v>
       </c>
       <c r="K7" s="10" t="s">
         <v>7</v>
@@ -2939,15 +3797,15 @@
       <c r="O7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="P7" s="22" t="s">
-        <v>60</v>
+      <c r="P7" s="20" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="19" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="10">
@@ -2963,7 +3821,7 @@
         <v>39</v>
       </c>
       <c r="I8" s="10"/>
-      <c r="J8" s="24"/>
+      <c r="J8" s="22"/>
       <c r="K8" s="10" t="s">
         <v>7</v>
       </c>
@@ -2979,13 +3837,13 @@
       <c r="O8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="P8" s="22" t="s">
+      <c r="P8" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>6</v>
@@ -3003,8 +3861,8 @@
         <v>38</v>
       </c>
       <c r="I9" s="10"/>
-      <c r="J9" s="24" t="s">
-        <v>54</v>
+      <c r="J9" s="22" t="s">
+        <v>52</v>
       </c>
       <c r="K9" s="10" t="s">
         <v>7</v>
@@ -3022,12 +3880,12 @@
         <v>7</v>
       </c>
       <c r="P9" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>3</v>
@@ -3045,7 +3903,7 @@
         <v>39</v>
       </c>
       <c r="I10" s="10"/>
-      <c r="J10" s="24"/>
+      <c r="J10" s="22"/>
       <c r="K10" s="10" t="s">
         <v>7</v>
       </c>
@@ -3062,12 +3920,12 @@
         <v>7</v>
       </c>
       <c r="P10" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>12</v>
@@ -3081,8 +3939,8 @@
         <v>39</v>
       </c>
       <c r="I11" s="10"/>
-      <c r="J11" s="24" t="s">
-        <v>54</v>
+      <c r="J11" s="22" t="s">
+        <v>52</v>
       </c>
       <c r="K11" s="10" t="s">
         <v>7</v>
@@ -3100,12 +3958,12 @@
         <v>7</v>
       </c>
       <c r="P11" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>12</v>
@@ -3119,8 +3977,8 @@
         <v>39</v>
       </c>
       <c r="I12" s="10"/>
-      <c r="J12" s="24" t="s">
-        <v>54</v>
+      <c r="J12" s="22" t="s">
+        <v>52</v>
       </c>
       <c r="K12" s="10" t="s">
         <v>7</v>
@@ -3138,12 +3996,12 @@
         <v>7</v>
       </c>
       <c r="P12" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>3</v>
@@ -3161,8 +4019,8 @@
         <v>39</v>
       </c>
       <c r="I13" s="10"/>
-      <c r="J13" s="24" t="s">
-        <v>54</v>
+      <c r="J13" s="22" t="s">
+        <v>52</v>
       </c>
       <c r="K13" s="10" t="s">
         <v>7</v>
@@ -3180,12 +4038,12 @@
         <v>7</v>
       </c>
       <c r="P13" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>3</v>
@@ -3203,8 +4061,8 @@
         <v>39</v>
       </c>
       <c r="I14" s="10"/>
-      <c r="J14" s="24" t="s">
-        <v>54</v>
+      <c r="J14" s="22" t="s">
+        <v>52</v>
       </c>
       <c r="K14" s="10" t="s">
         <v>4</v>
@@ -3222,12 +4080,12 @@
         <v>7</v>
       </c>
       <c r="P14" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>6</v>
@@ -3245,7 +4103,7 @@
         <v>39</v>
       </c>
       <c r="I15" s="10"/>
-      <c r="J15" s="24"/>
+      <c r="J15" s="22"/>
       <c r="K15" s="10" t="s">
         <v>4</v>
       </c>
@@ -3262,15 +4120,15 @@
         <v>7</v>
       </c>
       <c r="P15" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -3278,31 +4136,31 @@
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="I16" s="39">
+        <v>105</v>
+      </c>
+      <c r="I16" s="35">
         <v>0</v>
       </c>
       <c r="J16" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="K16" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="L16" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="M16" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="N16" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="O16" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="P16" s="7" t="s">
         <v>108</v>
-      </c>
-      <c r="K16" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="L16" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="M16" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="N16" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="O16" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="P16" s="7" t="s">
-        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -3349,10 +4207,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D607A43C-CF77-4FEB-8267-E2A8E14E5F12}">
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3376,76 +4234,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
-      <c r="O1" s="42"/>
-      <c r="P1" s="42"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="str">
         <f>'Objeto de dominio'!A1&amp;":"</f>
         <v>Objeto de dominio:</v>
       </c>
-      <c r="B2" s="53" t="str">
+      <c r="B2" s="50" t="str">
         <f>'Objeto de dominio'!A3&amp;":"</f>
         <v>Conductor:</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="55"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="51"/>
+      <c r="P2" s="52"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="str">
         <f>'Objeto de dominio'!B1&amp;":"</f>
         <v>Descripcion:</v>
       </c>
-      <c r="B3" s="56" t="str">
+      <c r="B3" s="53" t="str">
         <f>'Objeto de dominio'!B3</f>
         <v>Usuario encargadode realizar las rutas, es quien crea y da los detalles de cuando y por donde pasa, para así poder transportar a otros usuarios. El conductor tiene un vehiculo el cual dispone para compartir y generar ganacias de trasportar otros usuarios.</v>
       </c>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="57"/>
-      <c r="N3" s="57"/>
-      <c r="O3" s="57"/>
-      <c r="P3" s="58"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="54"/>
+      <c r="P3" s="55"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
@@ -3570,7 +4428,7 @@
       </c>
       <c r="I7" s="10"/>
       <c r="J7" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K7" s="10" t="s">
         <v>7</v>
@@ -3652,7 +4510,7 @@
       </c>
       <c r="I9" s="10"/>
       <c r="J9" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K9" s="10" t="s">
         <v>7</v>
@@ -3670,12 +4528,12 @@
         <v>7</v>
       </c>
       <c r="P9" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>3</v>
@@ -3694,7 +4552,7 @@
       </c>
       <c r="I10" s="10"/>
       <c r="J10" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K10" s="10" t="s">
         <v>7</v>
@@ -3712,7 +4570,7 @@
         <v>7</v>
       </c>
       <c r="P10" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="30" x14ac:dyDescent="0.25">
@@ -3736,7 +4594,7 @@
       </c>
       <c r="I11" s="10"/>
       <c r="J11" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K11" s="10" t="s">
         <v>7</v>
@@ -3754,15 +4612,15 @@
         <v>7</v>
       </c>
       <c r="P11" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>75</v>
+        <v>73</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>73</v>
       </c>
       <c r="C12" s="10">
         <v>0</v>
@@ -3794,7 +4652,45 @@
         <v>7</v>
       </c>
       <c r="P12" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="O13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="P13" s="7" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -3816,13 +4712,13 @@
           <x14:formula1>
             <xm:f>Valores!$A$2:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>B6:B11</xm:sqref>
+          <xm:sqref>B6:B11 B13</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{33B96184-27A3-4839-87D1-3FEA800048F6}">
           <x14:formula1>
             <xm:f>Valores!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>K6:O12</xm:sqref>
+          <xm:sqref>K6:O13</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Creacion de datos simulados
</commit_message>
<xml_diff>
--- a/ExtraClase/Modelado de Dominio/Modelo enriquesido/Proyecto extraclase.xlsx
+++ b/ExtraClase/Modelado de Dominio/Modelo enriquesido/Proyecto extraclase.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Federico\U\Doo\RepositorioDOO\ExtraClase\Modelado de Dominio\Modelo enriquesido\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1190F4E0-1C25-47A5-97A9-498AFA784A93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B1CB114-B5E8-42FA-92C2-9547E270245E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="3" xr2:uid="{91EDD603-1B87-409C-9594-5C05F8123E08}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="6" activeTab="7" xr2:uid="{91EDD603-1B87-409C-9594-5C05F8123E08}"/>
   </bookViews>
   <sheets>
     <sheet name="Valores" sheetId="1" r:id="rId1"/>
-    <sheet name="Modelo de dominio" sheetId="2" state="hidden" r:id="rId2"/>
+    <sheet name="Modelo de dominio" sheetId="2" r:id="rId2"/>
     <sheet name="Objeto de dominio" sheetId="3" r:id="rId3"/>
     <sheet name="Conductor Vehiculo" sheetId="15" r:id="rId4"/>
     <sheet name="Calificación" sheetId="9" state="hidden" r:id="rId5"/>
@@ -993,71 +993,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1069,34 +1004,99 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="6" fillId="8" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1569,92 +1569,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="str">
         <f>'Objeto de dominio'!A1&amp;":"</f>
         <v>Objeto de dominio:</v>
       </c>
-      <c r="B2" s="61" t="str">
+      <c r="B2" s="70" t="str">
         <f>'Objeto de dominio'!A2&amp;":"</f>
         <v>Clientes:</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62"/>
-      <c r="L2" s="62"/>
-      <c r="M2" s="62"/>
-      <c r="N2" s="62"/>
-      <c r="O2" s="62"/>
-      <c r="P2" s="63"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
+      <c r="O2" s="71"/>
+      <c r="P2" s="72"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="str">
         <f>'Objeto de dominio'!B1&amp;":"</f>
         <v>Descripcion:</v>
       </c>
-      <c r="B3" s="64" t="str">
+      <c r="B3" s="73" t="str">
         <f>'Objeto de dominio'!B7</f>
         <v>Objeto que nos representa cuales son las rutas que se da en un viaje, como lo puede ser, por donde pasa, quienes estuvieron en el viaje y hasta donde llegaron, se busca es guardar daros por seguridad de los usuarios.</v>
       </c>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
-      <c r="L3" s="65"/>
-      <c r="M3" s="65"/>
-      <c r="N3" s="65"/>
-      <c r="O3" s="65"/>
-      <c r="P3" s="66"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="74"/>
+      <c r="K3" s="74"/>
+      <c r="L3" s="74"/>
+      <c r="M3" s="74"/>
+      <c r="N3" s="74"/>
+      <c r="O3" s="74"/>
+      <c r="P3" s="75"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="76" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="68"/>
-      <c r="C4" s="68"/>
-      <c r="D4" s="68"/>
-      <c r="E4" s="68"/>
-      <c r="F4" s="68"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="68"/>
-      <c r="I4" s="68"/>
-      <c r="J4" s="68"/>
-      <c r="K4" s="68"/>
-      <c r="L4" s="68"/>
-      <c r="M4" s="68"/>
-      <c r="N4" s="68"/>
-      <c r="O4" s="68"/>
-      <c r="P4" s="69"/>
+      <c r="B4" s="77"/>
+      <c r="C4" s="77"/>
+      <c r="D4" s="77"/>
+      <c r="E4" s="77"/>
+      <c r="F4" s="77"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="77"/>
+      <c r="I4" s="77"/>
+      <c r="J4" s="77"/>
+      <c r="K4" s="77"/>
+      <c r="L4" s="77"/>
+      <c r="M4" s="77"/>
+      <c r="N4" s="77"/>
+      <c r="O4" s="77"/>
+      <c r="P4" s="78"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -2217,72 +2217,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="str">
         <f>'Objeto de dominio'!A1&amp;":"</f>
         <v>Objeto de dominio:</v>
       </c>
-      <c r="B2" s="61" t="str">
+      <c r="B2" s="70" t="str">
         <f>'Objeto de dominio'!A3&amp;":"</f>
         <v>Conductor:</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62"/>
-      <c r="L2" s="62"/>
-      <c r="M2" s="62"/>
-      <c r="N2" s="62"/>
-      <c r="O2" s="62"/>
-      <c r="P2" s="63"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
+      <c r="O2" s="71"/>
+      <c r="P2" s="72"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="str">
         <f>'Objeto de dominio'!B1&amp;":"</f>
         <v>Descripcion:</v>
       </c>
-      <c r="B3" s="64" t="str">
+      <c r="B3" s="73" t="str">
         <f>'Objeto de dominio'!B3</f>
         <v>Usuario encargadode realizar las rutas, es quien crea y da los detalles de cuando y por donde pasa, para así poder transportar a otros usuarios. El conductor tiene un vehiculo el cual dispone para compartir y generar ganacias de trasportar otros usuarios.</v>
       </c>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
-      <c r="L3" s="65"/>
-      <c r="M3" s="65"/>
-      <c r="N3" s="65"/>
-      <c r="O3" s="65"/>
-      <c r="P3" s="66"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="74"/>
+      <c r="K3" s="74"/>
+      <c r="L3" s="74"/>
+      <c r="M3" s="74"/>
+      <c r="N3" s="74"/>
+      <c r="O3" s="74"/>
+      <c r="P3" s="75"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
@@ -2715,7 +2715,7 @@
   <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:P3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="56.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2739,72 +2739,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="59" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="str">
         <f>'Objeto de dominio'!A1&amp;":"</f>
         <v>Objeto de dominio:</v>
       </c>
-      <c r="B2" s="53" t="str">
+      <c r="B2" s="79" t="str">
         <f>'Objeto de dominio'!A8&amp;":"</f>
         <v>Ubicación:</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="55"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
+      <c r="O2" s="80"/>
+      <c r="P2" s="81"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="str">
         <f>'Objeto de dominio'!B1&amp;":"</f>
         <v>Descripcion:</v>
       </c>
-      <c r="B3" s="70" t="str">
+      <c r="B3" s="82" t="str">
         <f>'Objeto de dominio'!B8</f>
         <v>Objeto que representa cual será el lugar geografico de un cliente o un conductor al momento de registrar un servicio, como lo puede ser una ciudad, barrio o sesctor. Por ejemplo un cliente puede estar en la ciudad rionegro en el barrio villa Manuela.</v>
       </c>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="70"/>
-      <c r="K3" s="70"/>
-      <c r="L3" s="70"/>
-      <c r="M3" s="70"/>
-      <c r="N3" s="70"/>
-      <c r="O3" s="70"/>
-      <c r="P3" s="70"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="82"/>
+      <c r="L3" s="82"/>
+      <c r="M3" s="82"/>
+      <c r="N3" s="82"/>
+      <c r="O3" s="82"/>
+      <c r="P3" s="82"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
@@ -3266,92 +3266,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="59" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="str">
         <f>'Objeto de dominio'!A1&amp;":"</f>
         <v>Objeto de dominio:</v>
       </c>
-      <c r="B2" s="53" t="str">
+      <c r="B2" s="79" t="str">
         <f>'Objeto de dominio'!A2&amp;":"</f>
         <v>Clientes:</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="55"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
+      <c r="O2" s="80"/>
+      <c r="P2" s="81"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="str">
         <f>'Objeto de dominio'!B1&amp;":"</f>
         <v>Descripcion:</v>
       </c>
-      <c r="B3" s="52" t="str">
+      <c r="B3" s="83" t="str">
         <f>'Objeto de dominio'!B2</f>
         <v>Objeto que representa a un tipo de usuario, el cual es quien solicita el servicio de carro compartido. Por ejmeplo es quien contacta con un conductor para llegar a un destino en común.</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="52"/>
-      <c r="M3" s="52"/>
-      <c r="N3" s="52"/>
-      <c r="O3" s="52"/>
-      <c r="P3" s="52"/>
-    </row>
-    <row r="4" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="56" t="s">
+      <c r="C3" s="83"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="83"/>
+      <c r="F3" s="83"/>
+      <c r="G3" s="83"/>
+      <c r="H3" s="83"/>
+      <c r="I3" s="83"/>
+      <c r="J3" s="83"/>
+      <c r="K3" s="83"/>
+      <c r="L3" s="83"/>
+      <c r="M3" s="83"/>
+      <c r="N3" s="83"/>
+      <c r="O3" s="83"/>
+      <c r="P3" s="83"/>
+    </row>
+    <row r="4" spans="1:16" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="57"/>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
-      <c r="E4" s="57"/>
-      <c r="F4" s="57"/>
-      <c r="G4" s="57"/>
-      <c r="H4" s="57"/>
-      <c r="I4" s="57"/>
-      <c r="J4" s="57"/>
-      <c r="K4" s="57"/>
-      <c r="L4" s="57"/>
-      <c r="M4" s="57"/>
-      <c r="N4" s="57"/>
-      <c r="O4" s="57"/>
-      <c r="P4" s="57"/>
+      <c r="B4" s="85"/>
+      <c r="C4" s="85"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="85"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="85"/>
+      <c r="I4" s="85"/>
+      <c r="J4" s="85"/>
+      <c r="K4" s="85"/>
+      <c r="L4" s="85"/>
+      <c r="M4" s="85"/>
+      <c r="N4" s="85"/>
+      <c r="O4" s="85"/>
+      <c r="P4" s="85"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -3679,8 +3679,8 @@
   <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3695,13 +3695,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="50" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
       <c r="F1" s="23"/>
       <c r="G1" s="23"/>
       <c r="H1" s="23"/>
@@ -3715,16 +3715,16 @@
       <c r="P1" s="23"/>
     </row>
     <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="87" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
+      <c r="B2" s="87"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="87"/>
       <c r="I2" s="23"/>
       <c r="J2" s="23"/>
       <c r="K2" s="23"/>
@@ -3735,23 +3735,23 @@
       <c r="P2" s="23"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="75" t="str">
+      <c r="A3" s="52" t="str">
         <f>Cliente!A6</f>
         <v>Codigo</v>
       </c>
-      <c r="B3" s="75" t="str">
+      <c r="B3" s="52" t="str">
         <f>Cliente!A7</f>
         <v>Nombre</v>
       </c>
-      <c r="C3" s="75" t="str">
+      <c r="C3" s="52" t="str">
         <f>Ubicacion!A8</f>
         <v>Ciudad</v>
       </c>
-      <c r="D3" s="75" t="str">
+      <c r="D3" s="52" t="str">
         <f>Ubicacion!A9</f>
         <v>Barrio o sector</v>
       </c>
-      <c r="E3" s="75" t="str">
+      <c r="E3" s="52" t="str">
         <f>Ubicacion!A10</f>
         <v>Hora</v>
       </c>
@@ -3769,19 +3769,19 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="76">
+      <c r="A4" s="53">
         <v>1</v>
       </c>
-      <c r="B4" s="76" t="s">
+      <c r="B4" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="76" t="s">
+      <c r="C4" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="76" t="s">
+      <c r="D4" s="53" t="s">
         <v>126</v>
       </c>
-      <c r="E4" s="77">
+      <c r="E4" s="54">
         <v>0.54166666666666663</v>
       </c>
       <c r="F4" s="46"/>
@@ -3791,16 +3791,16 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="78" t="s">
+      <c r="A6" s="87" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="79"/>
-      <c r="C6" s="79"/>
-      <c r="D6" s="79"/>
-      <c r="E6" s="79"/>
-      <c r="F6" s="79"/>
-      <c r="G6" s="79"/>
-      <c r="H6" s="79"/>
+      <c r="B6" s="88"/>
+      <c r="C6" s="88"/>
+      <c r="D6" s="88"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="88"/>
+      <c r="G6" s="88"/>
+      <c r="H6" s="88"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="45" t="str">
@@ -3863,14 +3863,14 @@
       </c>
     </row>
     <row r="10" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="78" t="s">
+      <c r="A10" s="87" t="s">
         <v>84</v>
       </c>
-      <c r="B10" s="78"/>
-      <c r="C10" s="78"/>
-      <c r="D10" s="78"/>
-      <c r="E10" s="78"/>
-      <c r="F10" s="78"/>
+      <c r="B10" s="87"/>
+      <c r="C10" s="87"/>
+      <c r="D10" s="87"/>
+      <c r="E10" s="87"/>
+      <c r="F10" s="87"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="45" t="str">
@@ -3976,8 +3976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA3A2587-FA68-46BD-83B7-0F0FB56FF0F2}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3993,10 +3993,10 @@
       <c r="B1" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="80" t="s">
+      <c r="C1" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="81"/>
+      <c r="D1" s="58"/>
     </row>
     <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
@@ -4103,7 +4103,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AAB3554-9B32-4CE9-9788-4B24092013FF}">
   <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -4128,92 +4128,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="59" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="86" t="str">
+      <c r="A2" s="56" t="str">
         <f>'Objeto de dominio'!A1&amp;":"</f>
         <v>Objeto de dominio:</v>
       </c>
-      <c r="B2" s="87" t="str">
+      <c r="B2" s="60" t="str">
         <f>'Objeto de dominio'!A11&amp;":"</f>
         <v>Conductor Vehiculo:</v>
       </c>
-      <c r="C2" s="87"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="87"/>
-      <c r="H2" s="87"/>
-      <c r="I2" s="87"/>
-      <c r="J2" s="87"/>
-      <c r="K2" s="87"/>
-      <c r="L2" s="87"/>
-      <c r="M2" s="87"/>
-      <c r="N2" s="87"/>
-      <c r="O2" s="87"/>
-      <c r="P2" s="87"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="60"/>
+      <c r="N2" s="60"/>
+      <c r="O2" s="60"/>
+      <c r="P2" s="60"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="86" t="str">
+      <c r="A3" s="56" t="str">
         <f>'Objeto de dominio'!B1&amp;":"</f>
         <v>Descripcion:</v>
       </c>
-      <c r="B3" s="88" t="str">
+      <c r="B3" s="61" t="str">
         <f>'Objeto de dominio'!B11</f>
         <v>Objeto que tiene la funcion de especificar quien es el conductor de que vehiculo, facilitando a los clientes para tomar la decisión de que ruta y vehiculo usar.</v>
       </c>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
-      <c r="H3" s="88"/>
-      <c r="I3" s="88"/>
-      <c r="J3" s="88"/>
-      <c r="K3" s="88"/>
-      <c r="L3" s="88"/>
-      <c r="M3" s="88"/>
-      <c r="N3" s="88"/>
-      <c r="O3" s="88"/>
-      <c r="P3" s="88"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="61"/>
+      <c r="L3" s="61"/>
+      <c r="M3" s="61"/>
+      <c r="N3" s="61"/>
+      <c r="O3" s="61"/>
+      <c r="P3" s="61"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="72"/>
-      <c r="D4" s="72"/>
-      <c r="E4" s="72"/>
-      <c r="F4" s="72"/>
-      <c r="G4" s="72"/>
-      <c r="H4" s="72"/>
-      <c r="I4" s="72"/>
-      <c r="J4" s="72"/>
-      <c r="K4" s="72"/>
-      <c r="L4" s="72"/>
-      <c r="M4" s="72"/>
-      <c r="N4" s="72"/>
-      <c r="O4" s="72"/>
-      <c r="P4" s="72"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="49"/>
+      <c r="M4" s="49"/>
+      <c r="N4" s="49"/>
+      <c r="O4" s="49"/>
+      <c r="P4" s="49"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -4446,92 +4446,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="59" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="str">
         <f>'Objeto de dominio'!A1&amp;":"</f>
         <v>Objeto de dominio:</v>
       </c>
-      <c r="B2" s="48" t="str">
+      <c r="B2" s="62" t="str">
         <f>'Objeto de dominio'!A4</f>
         <v>Calificación</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="48"/>
-      <c r="N2" s="48"/>
-      <c r="O2" s="48"/>
-      <c r="P2" s="48"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
+      <c r="L2" s="62"/>
+      <c r="M2" s="62"/>
+      <c r="N2" s="62"/>
+      <c r="O2" s="62"/>
+      <c r="P2" s="62"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="str">
         <f>'Objeto de dominio'!B1&amp;":"</f>
         <v>Descripcion:</v>
       </c>
-      <c r="B3" s="49" t="str">
+      <c r="B3" s="63" t="str">
         <f>'Objeto de dominio'!B4</f>
         <v>Objeto que representa cual es la calificacion conforme al servicio que recibio por parte del conductor, esta calificacion es general, toma en cuenta la actitud del conductor principalmente.</v>
       </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="49"/>
-      <c r="J3" s="49"/>
-      <c r="K3" s="49"/>
-      <c r="L3" s="49"/>
-      <c r="M3" s="49"/>
-      <c r="N3" s="49"/>
-      <c r="O3" s="49"/>
-      <c r="P3" s="49"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="63"/>
+      <c r="M3" s="63"/>
+      <c r="N3" s="63"/>
+      <c r="O3" s="63"/>
+      <c r="P3" s="63"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="51"/>
-      <c r="L4" s="51"/>
-      <c r="M4" s="51"/>
-      <c r="N4" s="51"/>
-      <c r="O4" s="51"/>
-      <c r="P4" s="51"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="64"/>
+      <c r="K4" s="64"/>
+      <c r="L4" s="64"/>
+      <c r="M4" s="64"/>
+      <c r="N4" s="64"/>
+      <c r="O4" s="64"/>
+      <c r="P4" s="64"/>
     </row>
     <row r="5" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -4839,92 +4839,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="65" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-      <c r="N1" s="59"/>
-      <c r="O1" s="59"/>
-      <c r="P1" s="59"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="65"/>
+      <c r="N1" s="65"/>
+      <c r="O1" s="65"/>
+      <c r="P1" s="65"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="str">
         <f>'Objeto de dominio'!A1&amp;":"</f>
         <v>Objeto de dominio:</v>
       </c>
-      <c r="B2" s="60" t="str">
+      <c r="B2" s="66" t="str">
         <f>'Objeto de dominio'!A5</f>
         <v>Vehiculo</v>
       </c>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
-      <c r="N2" s="60"/>
-      <c r="O2" s="60"/>
-      <c r="P2" s="60"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="66"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="66"/>
+      <c r="N2" s="66"/>
+      <c r="O2" s="66"/>
+      <c r="P2" s="66"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="str">
         <f>'Objeto de dominio'!B1&amp;":"</f>
         <v>Descripcion:</v>
       </c>
-      <c r="B3" s="60" t="str">
+      <c r="B3" s="66" t="str">
         <f>'Objeto de dominio'!B5</f>
         <v>Objeto que se encarga de identificar al vehiculo del conductor y a su vez el dueño</v>
       </c>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
-      <c r="M3" s="60"/>
-      <c r="N3" s="60"/>
-      <c r="O3" s="60"/>
-      <c r="P3" s="60"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
+      <c r="J3" s="66"/>
+      <c r="K3" s="66"/>
+      <c r="L3" s="66"/>
+      <c r="M3" s="66"/>
+      <c r="N3" s="66"/>
+      <c r="O3" s="66"/>
+      <c r="P3" s="66"/>
     </row>
     <row r="4" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="64" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="51"/>
-      <c r="L4" s="51"/>
-      <c r="M4" s="51"/>
-      <c r="N4" s="51"/>
-      <c r="O4" s="51"/>
-      <c r="P4" s="51"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="64"/>
+      <c r="K4" s="64"/>
+      <c r="L4" s="64"/>
+      <c r="M4" s="64"/>
+      <c r="N4" s="64"/>
+      <c r="O4" s="64"/>
+      <c r="P4" s="64"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -5167,72 +5167,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="59" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="str">
         <f>'Objeto de dominio'!A1&amp;":"</f>
         <v>Objeto de dominio:</v>
       </c>
-      <c r="B2" s="84" t="str">
+      <c r="B2" s="67" t="str">
         <f>'Objeto de dominio'!A10&amp;":"</f>
         <v>Peticion ruta:</v>
       </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
-      <c r="O2" s="84"/>
-      <c r="P2" s="84"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="67"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="67"/>
+      <c r="O2" s="67"/>
+      <c r="P2" s="67"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="str">
         <f>'Objeto de dominio'!B1&amp;":"</f>
         <v>Descripcion:</v>
       </c>
-      <c r="B3" s="85" t="str">
+      <c r="B3" s="68" t="str">
         <f>'Objeto de dominio'!B10</f>
         <v>Objeto con el cual un cliente puede hacer una solicitud para guardar el cupo en una reuta especifica, con la cual un conductor puede ver cuales clientes acepta o no para compartir su ruta</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
-      <c r="O3" s="85"/>
-      <c r="P3" s="85"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
+      <c r="L3" s="68"/>
+      <c r="M3" s="68"/>
+      <c r="N3" s="68"/>
+      <c r="O3" s="68"/>
+      <c r="P3" s="68"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="47" t="s">
@@ -5493,7 +5493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92D61B2C-9599-4A4E-A00B-69FF1717B2B8}">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
@@ -5518,72 +5518,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="65" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-      <c r="N1" s="59"/>
-      <c r="O1" s="59"/>
-      <c r="P1" s="59"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="65"/>
+      <c r="N1" s="65"/>
+      <c r="O1" s="65"/>
+      <c r="P1" s="65"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="str">
         <f>'Objeto de dominio'!A1&amp;":"</f>
         <v>Objeto de dominio:</v>
       </c>
-      <c r="B2" s="60" t="str">
+      <c r="B2" s="66" t="str">
         <f>'Objeto de dominio'!A6</f>
         <v>Detalle Ruta</v>
       </c>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
-      <c r="N2" s="60"/>
-      <c r="O2" s="60"/>
-      <c r="P2" s="60"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="66"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="66"/>
+      <c r="N2" s="66"/>
+      <c r="O2" s="66"/>
+      <c r="P2" s="66"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="str">
         <f>'Objeto de dominio'!B1&amp;":"</f>
         <v>Descripcion:</v>
       </c>
-      <c r="B3" s="60" t="str">
+      <c r="B3" s="66" t="str">
         <f>'Objeto de dominio'!B6</f>
         <v>Objeto que se encarga de guardar todo el recorrido de la ruta que hace el conductor en su vehiculo</v>
       </c>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
-      <c r="M3" s="60"/>
-      <c r="N3" s="60"/>
-      <c r="O3" s="60"/>
-      <c r="P3" s="60"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
+      <c r="J3" s="66"/>
+      <c r="K3" s="66"/>
+      <c r="L3" s="66"/>
+      <c r="M3" s="66"/>
+      <c r="N3" s="66"/>
+      <c r="O3" s="66"/>
+      <c r="P3" s="66"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">
@@ -5725,58 +5725,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="59" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="82" t="str">
+      <c r="A2" s="55" t="str">
         <f>'Objeto de dominio'!A1&amp;":"</f>
         <v>Objeto de dominio:</v>
       </c>
-      <c r="B2" s="82" t="str">
+      <c r="B2" s="55" t="str">
         <f>'Objeto de dominio'!A9</f>
         <v>Tipo vehiculo</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="82" t="str">
+      <c r="A3" s="55" t="str">
         <f>'Objeto de dominio'!B1&amp;":"</f>
         <v>Descripcion:</v>
       </c>
-      <c r="B3" s="83" t="str">
+      <c r="B3" s="69" t="str">
         <f>'Objeto de dominio'!B9</f>
         <v>Obejeto que descripbe con exactitud que tipo de medio trasporte se va utilizar, como lo puede ser que sea tipo motocicleta o tipo automovil.</v>
       </c>
-      <c r="C3" s="83"/>
-      <c r="D3" s="83"/>
-      <c r="E3" s="83"/>
-      <c r="F3" s="83"/>
-      <c r="G3" s="83"/>
-      <c r="H3" s="83"/>
-      <c r="I3" s="83"/>
-      <c r="J3" s="83"/>
-      <c r="K3" s="83"/>
-      <c r="L3" s="83"/>
-      <c r="M3" s="83"/>
-      <c r="N3" s="83"/>
-      <c r="O3" s="83"/>
-      <c r="P3" s="83"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="69"/>
+      <c r="K3" s="69"/>
+      <c r="L3" s="69"/>
+      <c r="M3" s="69"/>
+      <c r="N3" s="69"/>
+      <c r="O3" s="69"/>
+      <c r="P3" s="69"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">

</xml_diff>